<commit_message>
Added IBM Results, no calculation yet
</commit_message>
<xml_diff>
--- a/Datasets/Analysed Dataset (.csv, no calc)/MeaningCloud/MC_Analysed_Uber.xlsx
+++ b/Datasets/Analysed Dataset (.csv, no calc)/MeaningCloud/MC_Analysed_Uber.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QuangDaoVuNgoc\github\bachelorthesis\Datasets\Analysed Dataset (.csv, no calc)\MeaningCloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1074724F-ABC5-4186-9E2C-003DBE4610DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CB1343-C1C3-4D20-A681-4773312B545F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5118" uniqueCount="1359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5119" uniqueCount="1359">
   <si>
     <t>Polarity</t>
   </si>
@@ -4572,8 +4572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C938"/>
   <sheetViews>
-    <sheetView topLeftCell="A901" workbookViewId="0">
-      <selection activeCell="D928" sqref="D928"/>
+    <sheetView tabSelected="1" topLeftCell="A904" workbookViewId="0">
+      <selection activeCell="A939" sqref="A939"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14903,156 +14903,159 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C538F1-BFB8-49D4-8171-3A25C9325FC7}">
-  <dimension ref="A1:B404"/>
+  <dimension ref="A1:C405"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>-1</v>
       </c>
       <c r="B1" t="s">
+        <v>939</v>
+      </c>
+      <c r="C1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>-1</v>
+      </c>
+      <c r="B2" t="s">
         <v>940</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>-1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>-1</v>
+      </c>
+      <c r="B3" t="s">
         <v>941</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>-1</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>-1</v>
+      </c>
+      <c r="B4" t="s">
         <v>942</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>-1</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>-1</v>
+      </c>
+      <c r="B5" t="s">
         <v>943</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>-1</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>-1</v>
+      </c>
+      <c r="B6" t="s">
         <v>944</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>-1</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>-1</v>
+      </c>
+      <c r="B7" t="s">
         <v>945</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>-1</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>-1</v>
+      </c>
+      <c r="B8" t="s">
         <v>946</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>-1</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>-1</v>
+      </c>
+      <c r="B9" t="s">
         <v>947</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>-1</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>-1</v>
+      </c>
+      <c r="B10" t="s">
         <v>948</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>-1</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>-1</v>
+      </c>
+      <c r="B11" t="s">
         <v>949</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>-1</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>-1</v>
+      </c>
+      <c r="B12" t="s">
         <v>950</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
         <v>951</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
         <v>952</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
         <v>953</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>-1</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>-1</v>
+      </c>
+      <c r="B16" t="s">
         <v>954</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>-1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>955</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B17" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -15060,7 +15063,7 @@
         <v>-1</v>
       </c>
       <c r="B19" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -15068,7 +15071,7 @@
         <v>-1</v>
       </c>
       <c r="B20" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -15076,7 +15079,7 @@
         <v>-1</v>
       </c>
       <c r="B21" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -15084,7 +15087,7 @@
         <v>-1</v>
       </c>
       <c r="B22" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -15092,7 +15095,7 @@
         <v>-1</v>
       </c>
       <c r="B23" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -15100,39 +15103,39 @@
         <v>-1</v>
       </c>
       <c r="B24" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B25" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B27" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -15140,7 +15143,7 @@
         <v>-1</v>
       </c>
       <c r="B29" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -15148,23 +15151,23 @@
         <v>-1</v>
       </c>
       <c r="B30" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B31" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -15172,7 +15175,7 @@
         <v>-1</v>
       </c>
       <c r="B33" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -15180,7 +15183,7 @@
         <v>-1</v>
       </c>
       <c r="B34" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -15188,23 +15191,23 @@
         <v>-1</v>
       </c>
       <c r="B35" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B36" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -15212,7 +15215,7 @@
         <v>-1</v>
       </c>
       <c r="B38" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -15220,7 +15223,7 @@
         <v>-1</v>
       </c>
       <c r="B39" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -15228,7 +15231,7 @@
         <v>-1</v>
       </c>
       <c r="B40" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -15236,7 +15239,7 @@
         <v>-1</v>
       </c>
       <c r="B41" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -15244,7 +15247,7 @@
         <v>-1</v>
       </c>
       <c r="B42" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -15252,7 +15255,7 @@
         <v>-1</v>
       </c>
       <c r="B43" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -15260,7 +15263,7 @@
         <v>-1</v>
       </c>
       <c r="B44" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -15268,7 +15271,7 @@
         <v>-1</v>
       </c>
       <c r="B45" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -15276,7 +15279,7 @@
         <v>-1</v>
       </c>
       <c r="B46" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -15284,7 +15287,7 @@
         <v>-1</v>
       </c>
       <c r="B47" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -15292,7 +15295,7 @@
         <v>-1</v>
       </c>
       <c r="B48" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -15300,7 +15303,7 @@
         <v>-1</v>
       </c>
       <c r="B49" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -15308,7 +15311,7 @@
         <v>-1</v>
       </c>
       <c r="B50" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -15316,7 +15319,7 @@
         <v>-1</v>
       </c>
       <c r="B51" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -15324,7 +15327,7 @@
         <v>-1</v>
       </c>
       <c r="B52" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -15332,23 +15335,23 @@
         <v>-1</v>
       </c>
       <c r="B53" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B54" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B55" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -15356,23 +15359,23 @@
         <v>-1</v>
       </c>
       <c r="B56" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B57" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B58" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -15380,7 +15383,7 @@
         <v>-1</v>
       </c>
       <c r="B59" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -15388,7 +15391,7 @@
         <v>-1</v>
       </c>
       <c r="B60" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -15396,39 +15399,39 @@
         <v>-1</v>
       </c>
       <c r="B61" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B62" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B63" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B64" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B65" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -15436,7 +15439,7 @@
         <v>-1</v>
       </c>
       <c r="B66" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -15444,7 +15447,7 @@
         <v>-1</v>
       </c>
       <c r="B67" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -15452,7 +15455,7 @@
         <v>-1</v>
       </c>
       <c r="B68" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -15460,7 +15463,7 @@
         <v>-1</v>
       </c>
       <c r="B69" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -15468,23 +15471,23 @@
         <v>-1</v>
       </c>
       <c r="B70" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B71" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B72" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -15492,23 +15495,23 @@
         <v>-1</v>
       </c>
       <c r="B73" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B74" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B75" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -15516,7 +15519,7 @@
         <v>-1</v>
       </c>
       <c r="B76" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -15524,7 +15527,7 @@
         <v>-1</v>
       </c>
       <c r="B77" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -15532,7 +15535,7 @@
         <v>-1</v>
       </c>
       <c r="B78" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -15540,7 +15543,7 @@
         <v>-1</v>
       </c>
       <c r="B79" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -15548,7 +15551,7 @@
         <v>-1</v>
       </c>
       <c r="B80" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -15556,7 +15559,7 @@
         <v>-1</v>
       </c>
       <c r="B81" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -15564,39 +15567,39 @@
         <v>-1</v>
       </c>
       <c r="B82" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B83" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B84" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B85" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B86" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -15604,39 +15607,39 @@
         <v>-1</v>
       </c>
       <c r="B87" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B88" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B89" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B90" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B91" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -15644,7 +15647,7 @@
         <v>-1</v>
       </c>
       <c r="B92" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -15652,23 +15655,23 @@
         <v>-1</v>
       </c>
       <c r="B93" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B94" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B95" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -15676,7 +15679,7 @@
         <v>-1</v>
       </c>
       <c r="B96" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -15684,7 +15687,7 @@
         <v>-1</v>
       </c>
       <c r="B97" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -15692,7 +15695,7 @@
         <v>-1</v>
       </c>
       <c r="B98" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -15700,7 +15703,7 @@
         <v>-1</v>
       </c>
       <c r="B99" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -15708,7 +15711,7 @@
         <v>-1</v>
       </c>
       <c r="B100" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -15716,23 +15719,23 @@
         <v>-1</v>
       </c>
       <c r="B101" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B102" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B103" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -15740,7 +15743,7 @@
         <v>-1</v>
       </c>
       <c r="B104" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -15748,7 +15751,7 @@
         <v>-1</v>
       </c>
       <c r="B105" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -15756,7 +15759,7 @@
         <v>-1</v>
       </c>
       <c r="B106" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -15764,7 +15767,7 @@
         <v>-1</v>
       </c>
       <c r="B107" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -15772,7 +15775,7 @@
         <v>-1</v>
       </c>
       <c r="B108" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -15780,7 +15783,7 @@
         <v>-1</v>
       </c>
       <c r="B109" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -15788,7 +15791,7 @@
         <v>-1</v>
       </c>
       <c r="B110" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -15796,7 +15799,7 @@
         <v>-1</v>
       </c>
       <c r="B111" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -15804,7 +15807,7 @@
         <v>-1</v>
       </c>
       <c r="B112" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -15812,23 +15815,23 @@
         <v>-1</v>
       </c>
       <c r="B113" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B114" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B115" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -15836,7 +15839,7 @@
         <v>-1</v>
       </c>
       <c r="B116" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -15844,7 +15847,7 @@
         <v>-1</v>
       </c>
       <c r="B117" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -15852,7 +15855,7 @@
         <v>-1</v>
       </c>
       <c r="B118" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -15860,7 +15863,7 @@
         <v>-1</v>
       </c>
       <c r="B119" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -15868,7 +15871,7 @@
         <v>-1</v>
       </c>
       <c r="B120" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -15876,7 +15879,7 @@
         <v>-1</v>
       </c>
       <c r="B121" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -15884,7 +15887,7 @@
         <v>-1</v>
       </c>
       <c r="B122" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -15892,23 +15895,23 @@
         <v>-1</v>
       </c>
       <c r="B123" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B124" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B125" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -15916,7 +15919,7 @@
         <v>-1</v>
       </c>
       <c r="B126" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -15924,7 +15927,7 @@
         <v>-1</v>
       </c>
       <c r="B127" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -15932,7 +15935,7 @@
         <v>-1</v>
       </c>
       <c r="B128" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -15940,7 +15943,7 @@
         <v>-1</v>
       </c>
       <c r="B129" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -15948,7 +15951,7 @@
         <v>-1</v>
       </c>
       <c r="B130" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -15956,7 +15959,7 @@
         <v>-1</v>
       </c>
       <c r="B131" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -15964,7 +15967,7 @@
         <v>-1</v>
       </c>
       <c r="B132" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -15972,7 +15975,7 @@
         <v>-1</v>
       </c>
       <c r="B133" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -15980,23 +15983,23 @@
         <v>-1</v>
       </c>
       <c r="B134" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B135" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B136" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -16004,7 +16007,7 @@
         <v>-1</v>
       </c>
       <c r="B137" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -16012,7 +16015,7 @@
         <v>-1</v>
       </c>
       <c r="B138" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -16020,7 +16023,7 @@
         <v>-1</v>
       </c>
       <c r="B139" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -16028,7 +16031,7 @@
         <v>-1</v>
       </c>
       <c r="B140" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
@@ -16036,7 +16039,7 @@
         <v>-1</v>
       </c>
       <c r="B141" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -16044,7 +16047,7 @@
         <v>-1</v>
       </c>
       <c r="B142" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
@@ -16052,7 +16055,7 @@
         <v>-1</v>
       </c>
       <c r="B143" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
@@ -16060,7 +16063,7 @@
         <v>-1</v>
       </c>
       <c r="B144" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -16068,7 +16071,7 @@
         <v>-1</v>
       </c>
       <c r="B145" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
@@ -16076,7 +16079,7 @@
         <v>-1</v>
       </c>
       <c r="B146" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
@@ -16084,23 +16087,23 @@
         <v>-1</v>
       </c>
       <c r="B147" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B148" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B149" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
@@ -16108,7 +16111,7 @@
         <v>-1</v>
       </c>
       <c r="B150" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
@@ -16116,7 +16119,7 @@
         <v>-1</v>
       </c>
       <c r="B151" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
@@ -16124,7 +16127,7 @@
         <v>-1</v>
       </c>
       <c r="B152" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
@@ -16132,7 +16135,7 @@
         <v>-1</v>
       </c>
       <c r="B153" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -16140,7 +16143,7 @@
         <v>-1</v>
       </c>
       <c r="B154" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
@@ -16148,7 +16151,7 @@
         <v>-1</v>
       </c>
       <c r="B155" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
@@ -16156,23 +16159,23 @@
         <v>-1</v>
       </c>
       <c r="B156" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B157" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B158" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
@@ -16180,7 +16183,7 @@
         <v>-1</v>
       </c>
       <c r="B159" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
@@ -16188,7 +16191,7 @@
         <v>-1</v>
       </c>
       <c r="B160" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -16196,7 +16199,7 @@
         <v>-1</v>
       </c>
       <c r="B161" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
@@ -16204,7 +16207,7 @@
         <v>-1</v>
       </c>
       <c r="B162" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -16212,7 +16215,7 @@
         <v>-1</v>
       </c>
       <c r="B163" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
@@ -16220,7 +16223,7 @@
         <v>-1</v>
       </c>
       <c r="B164" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
@@ -16228,7 +16231,7 @@
         <v>-1</v>
       </c>
       <c r="B165" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
@@ -16236,15 +16239,15 @@
         <v>-1</v>
       </c>
       <c r="B166" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B167" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
@@ -16252,15 +16255,15 @@
         <v>1</v>
       </c>
       <c r="B168" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B169" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
@@ -16268,7 +16271,7 @@
         <v>-1</v>
       </c>
       <c r="B170" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
@@ -16276,7 +16279,7 @@
         <v>-1</v>
       </c>
       <c r="B171" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
@@ -16284,7 +16287,7 @@
         <v>-1</v>
       </c>
       <c r="B172" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
@@ -16292,7 +16295,7 @@
         <v>-1</v>
       </c>
       <c r="B173" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
@@ -16300,7 +16303,7 @@
         <v>-1</v>
       </c>
       <c r="B174" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
@@ -16308,23 +16311,23 @@
         <v>-1</v>
       </c>
       <c r="B175" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B176" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B177" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
@@ -16332,7 +16335,7 @@
         <v>-1</v>
       </c>
       <c r="B178" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
@@ -16340,7 +16343,7 @@
         <v>-1</v>
       </c>
       <c r="B179" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
@@ -16348,7 +16351,7 @@
         <v>-1</v>
       </c>
       <c r="B180" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
@@ -16356,7 +16359,7 @@
         <v>-1</v>
       </c>
       <c r="B181" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
@@ -16364,7 +16367,7 @@
         <v>-1</v>
       </c>
       <c r="B182" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
@@ -16372,23 +16375,23 @@
         <v>-1</v>
       </c>
       <c r="B183" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B184" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B185" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
@@ -16396,23 +16399,23 @@
         <v>-1</v>
       </c>
       <c r="B186" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B187" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B188" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
@@ -16420,7 +16423,7 @@
         <v>-1</v>
       </c>
       <c r="B189" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
@@ -16428,23 +16431,23 @@
         <v>-1</v>
       </c>
       <c r="B190" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B191" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B192" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
@@ -16452,15 +16455,15 @@
         <v>-1</v>
       </c>
       <c r="B193" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B194" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
@@ -16468,15 +16471,15 @@
         <v>1</v>
       </c>
       <c r="B195" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B196" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
@@ -16484,15 +16487,15 @@
         <v>-1</v>
       </c>
       <c r="B197" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B198" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
@@ -16500,15 +16503,15 @@
         <v>1</v>
       </c>
       <c r="B199" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B200" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
@@ -16516,15 +16519,15 @@
         <v>-1</v>
       </c>
       <c r="B201" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B202" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
@@ -16532,15 +16535,15 @@
         <v>1</v>
       </c>
       <c r="B203" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B204" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
@@ -16548,7 +16551,7 @@
         <v>-1</v>
       </c>
       <c r="B205" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
@@ -16556,7 +16559,7 @@
         <v>-1</v>
       </c>
       <c r="B206" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
@@ -16564,23 +16567,23 @@
         <v>-1</v>
       </c>
       <c r="B207" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B208" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B209" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
@@ -16588,7 +16591,7 @@
         <v>-1</v>
       </c>
       <c r="B210" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
@@ -16596,7 +16599,7 @@
         <v>-1</v>
       </c>
       <c r="B211" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
@@ -16604,7 +16607,7 @@
         <v>-1</v>
       </c>
       <c r="B212" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
@@ -16612,7 +16615,7 @@
         <v>-1</v>
       </c>
       <c r="B213" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
@@ -16620,7 +16623,7 @@
         <v>-1</v>
       </c>
       <c r="B214" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
@@ -16628,7 +16631,7 @@
         <v>-1</v>
       </c>
       <c r="B215" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
@@ -16636,7 +16639,7 @@
         <v>-1</v>
       </c>
       <c r="B216" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
@@ -16644,7 +16647,7 @@
         <v>-1</v>
       </c>
       <c r="B217" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
@@ -16652,7 +16655,7 @@
         <v>-1</v>
       </c>
       <c r="B218" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
@@ -16660,7 +16663,7 @@
         <v>-1</v>
       </c>
       <c r="B219" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
@@ -16668,23 +16671,23 @@
         <v>-1</v>
       </c>
       <c r="B220" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B221" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B222" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
@@ -16692,7 +16695,7 @@
         <v>-1</v>
       </c>
       <c r="B223" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
@@ -16700,7 +16703,7 @@
         <v>-1</v>
       </c>
       <c r="B224" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
@@ -16708,23 +16711,23 @@
         <v>-1</v>
       </c>
       <c r="B225" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B226" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B227" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
@@ -16732,7 +16735,7 @@
         <v>-1</v>
       </c>
       <c r="B228" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
@@ -16740,7 +16743,7 @@
         <v>-1</v>
       </c>
       <c r="B229" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
@@ -16748,7 +16751,7 @@
         <v>-1</v>
       </c>
       <c r="B230" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
@@ -16756,7 +16759,7 @@
         <v>-1</v>
       </c>
       <c r="B231" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
@@ -16764,7 +16767,7 @@
         <v>-1</v>
       </c>
       <c r="B232" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
@@ -16772,7 +16775,7 @@
         <v>-1</v>
       </c>
       <c r="B233" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
@@ -16780,7 +16783,7 @@
         <v>-1</v>
       </c>
       <c r="B234" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
@@ -16788,23 +16791,23 @@
         <v>-1</v>
       </c>
       <c r="B235" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B236" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B237" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
@@ -16812,7 +16815,7 @@
         <v>-1</v>
       </c>
       <c r="B238" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
@@ -16820,7 +16823,7 @@
         <v>-1</v>
       </c>
       <c r="B239" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
@@ -16828,7 +16831,7 @@
         <v>-1</v>
       </c>
       <c r="B240" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
@@ -16836,7 +16839,7 @@
         <v>-1</v>
       </c>
       <c r="B241" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
@@ -16844,7 +16847,7 @@
         <v>-1</v>
       </c>
       <c r="B242" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
@@ -16852,7 +16855,7 @@
         <v>-1</v>
       </c>
       <c r="B243" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
@@ -16860,7 +16863,7 @@
         <v>-1</v>
       </c>
       <c r="B244" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
@@ -16868,7 +16871,7 @@
         <v>-1</v>
       </c>
       <c r="B245" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
@@ -16876,7 +16879,7 @@
         <v>-1</v>
       </c>
       <c r="B246" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
@@ -16884,7 +16887,7 @@
         <v>-1</v>
       </c>
       <c r="B247" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
@@ -16892,7 +16895,7 @@
         <v>-1</v>
       </c>
       <c r="B248" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
@@ -16900,7 +16903,7 @@
         <v>-1</v>
       </c>
       <c r="B249" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
@@ -16908,7 +16911,7 @@
         <v>-1</v>
       </c>
       <c r="B250" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
@@ -16916,7 +16919,7 @@
         <v>-1</v>
       </c>
       <c r="B251" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
@@ -16924,7 +16927,7 @@
         <v>-1</v>
       </c>
       <c r="B252" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
@@ -16932,7 +16935,7 @@
         <v>-1</v>
       </c>
       <c r="B253" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
@@ -16940,23 +16943,23 @@
         <v>-1</v>
       </c>
       <c r="B254" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B255" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B256" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
@@ -16964,7 +16967,7 @@
         <v>-1</v>
       </c>
       <c r="B257" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
@@ -16972,7 +16975,7 @@
         <v>-1</v>
       </c>
       <c r="B258" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
@@ -16980,7 +16983,7 @@
         <v>-1</v>
       </c>
       <c r="B259" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
@@ -16988,7 +16991,7 @@
         <v>-1</v>
       </c>
       <c r="B260" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
@@ -16996,23 +16999,23 @@
         <v>-1</v>
       </c>
       <c r="B261" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B262" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B263" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
@@ -17020,7 +17023,7 @@
         <v>-1</v>
       </c>
       <c r="B264" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
@@ -17028,7 +17031,7 @@
         <v>-1</v>
       </c>
       <c r="B265" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
@@ -17036,7 +17039,7 @@
         <v>-1</v>
       </c>
       <c r="B266" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
@@ -17044,23 +17047,23 @@
         <v>-1</v>
       </c>
       <c r="B267" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B268" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B269" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
@@ -17068,7 +17071,7 @@
         <v>-1</v>
       </c>
       <c r="B270" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
@@ -17076,15 +17079,15 @@
         <v>-1</v>
       </c>
       <c r="B271" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B272" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
@@ -17092,15 +17095,15 @@
         <v>1</v>
       </c>
       <c r="B273" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B274" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
@@ -17108,23 +17111,23 @@
         <v>-1</v>
       </c>
       <c r="B275" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B276" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B277" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
@@ -17132,7 +17135,7 @@
         <v>-1</v>
       </c>
       <c r="B278" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
@@ -17140,7 +17143,7 @@
         <v>-1</v>
       </c>
       <c r="B279" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
@@ -17148,23 +17151,23 @@
         <v>-1</v>
       </c>
       <c r="B280" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B281" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B282" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
@@ -17172,7 +17175,7 @@
         <v>-1</v>
       </c>
       <c r="B283" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
@@ -17180,7 +17183,7 @@
         <v>-1</v>
       </c>
       <c r="B284" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
@@ -17188,7 +17191,7 @@
         <v>-1</v>
       </c>
       <c r="B285" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
@@ -17196,7 +17199,7 @@
         <v>-1</v>
       </c>
       <c r="B286" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
@@ -17204,7 +17207,7 @@
         <v>-1</v>
       </c>
       <c r="B287" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
@@ -17212,39 +17215,39 @@
         <v>-1</v>
       </c>
       <c r="B288" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B289" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B290" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B291" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B292" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
@@ -17252,7 +17255,7 @@
         <v>-1</v>
       </c>
       <c r="B293" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
@@ -17260,7 +17263,7 @@
         <v>-1</v>
       </c>
       <c r="B294" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
@@ -17268,7 +17271,7 @@
         <v>-1</v>
       </c>
       <c r="B295" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
@@ -17276,7 +17279,7 @@
         <v>-1</v>
       </c>
       <c r="B296" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
@@ -17284,7 +17287,7 @@
         <v>-1</v>
       </c>
       <c r="B297" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
@@ -17292,7 +17295,7 @@
         <v>-1</v>
       </c>
       <c r="B298" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
@@ -17300,7 +17303,7 @@
         <v>-1</v>
       </c>
       <c r="B299" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
@@ -17308,7 +17311,7 @@
         <v>-1</v>
       </c>
       <c r="B300" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
@@ -17316,7 +17319,7 @@
         <v>-1</v>
       </c>
       <c r="B301" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
@@ -17324,7 +17327,7 @@
         <v>-1</v>
       </c>
       <c r="B302" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
@@ -17332,7 +17335,7 @@
         <v>-1</v>
       </c>
       <c r="B303" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
@@ -17340,7 +17343,7 @@
         <v>-1</v>
       </c>
       <c r="B304" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
@@ -17348,23 +17351,23 @@
         <v>-1</v>
       </c>
       <c r="B305" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B306" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B307" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
@@ -17372,15 +17375,15 @@
         <v>-1</v>
       </c>
       <c r="B308" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B309" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
@@ -17388,15 +17391,15 @@
         <v>1</v>
       </c>
       <c r="B310" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B311" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
@@ -17404,7 +17407,7 @@
         <v>-1</v>
       </c>
       <c r="B312" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
@@ -17412,23 +17415,23 @@
         <v>-1</v>
       </c>
       <c r="B313" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B314" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B315" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
@@ -17436,7 +17439,7 @@
         <v>-1</v>
       </c>
       <c r="B316" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
@@ -17444,7 +17447,7 @@
         <v>-1</v>
       </c>
       <c r="B317" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
@@ -17452,7 +17455,7 @@
         <v>-1</v>
       </c>
       <c r="B318" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
@@ -17460,7 +17463,7 @@
         <v>-1</v>
       </c>
       <c r="B319" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
@@ -17468,7 +17471,7 @@
         <v>-1</v>
       </c>
       <c r="B320" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
@@ -17476,7 +17479,7 @@
         <v>-1</v>
       </c>
       <c r="B321" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
@@ -17484,7 +17487,7 @@
         <v>-1</v>
       </c>
       <c r="B322" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
@@ -17492,7 +17495,7 @@
         <v>-1</v>
       </c>
       <c r="B323" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
@@ -17500,7 +17503,7 @@
         <v>-1</v>
       </c>
       <c r="B324" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
@@ -17508,7 +17511,7 @@
         <v>-1</v>
       </c>
       <c r="B325" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
@@ -17516,7 +17519,7 @@
         <v>-1</v>
       </c>
       <c r="B326" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
@@ -17524,23 +17527,23 @@
         <v>-1</v>
       </c>
       <c r="B327" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A328">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B328" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A329">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B329" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
@@ -17548,7 +17551,7 @@
         <v>-1</v>
       </c>
       <c r="B330" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
@@ -17556,7 +17559,7 @@
         <v>-1</v>
       </c>
       <c r="B331" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
@@ -17564,7 +17567,7 @@
         <v>-1</v>
       </c>
       <c r="B332" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
@@ -17572,7 +17575,7 @@
         <v>-1</v>
       </c>
       <c r="B333" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
@@ -17580,7 +17583,7 @@
         <v>-1</v>
       </c>
       <c r="B334" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
@@ -17588,7 +17591,7 @@
         <v>-1</v>
       </c>
       <c r="B335" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
@@ -17596,23 +17599,23 @@
         <v>-1</v>
       </c>
       <c r="B336" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A337">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B337" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A338">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B338" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
@@ -17620,7 +17623,7 @@
         <v>-1</v>
       </c>
       <c r="B339" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
@@ -17628,7 +17631,7 @@
         <v>-1</v>
       </c>
       <c r="B340" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
@@ -17636,7 +17639,7 @@
         <v>-1</v>
       </c>
       <c r="B341" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
@@ -17644,7 +17647,7 @@
         <v>-1</v>
       </c>
       <c r="B342" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
@@ -17652,7 +17655,7 @@
         <v>-1</v>
       </c>
       <c r="B343" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
@@ -17660,7 +17663,7 @@
         <v>-1</v>
       </c>
       <c r="B344" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
@@ -17668,7 +17671,7 @@
         <v>-1</v>
       </c>
       <c r="B345" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
@@ -17676,7 +17679,7 @@
         <v>-1</v>
       </c>
       <c r="B346" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
@@ -17684,7 +17687,7 @@
         <v>-1</v>
       </c>
       <c r="B347" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.25">
@@ -17692,7 +17695,7 @@
         <v>-1</v>
       </c>
       <c r="B348" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
@@ -17700,7 +17703,7 @@
         <v>-1</v>
       </c>
       <c r="B349" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
@@ -17708,7 +17711,7 @@
         <v>-1</v>
       </c>
       <c r="B350" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
@@ -17716,7 +17719,7 @@
         <v>-1</v>
       </c>
       <c r="B351" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
@@ -17724,7 +17727,7 @@
         <v>-1</v>
       </c>
       <c r="B352" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.25">
@@ -17732,7 +17735,7 @@
         <v>-1</v>
       </c>
       <c r="B353" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.25">
@@ -17740,7 +17743,7 @@
         <v>-1</v>
       </c>
       <c r="B354" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
@@ -17748,7 +17751,7 @@
         <v>-1</v>
       </c>
       <c r="B355" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
@@ -17756,7 +17759,7 @@
         <v>-1</v>
       </c>
       <c r="B356" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.25">
@@ -17764,7 +17767,7 @@
         <v>-1</v>
       </c>
       <c r="B357" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
@@ -17772,7 +17775,7 @@
         <v>-1</v>
       </c>
       <c r="B358" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
@@ -17780,7 +17783,7 @@
         <v>-1</v>
       </c>
       <c r="B359" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
@@ -17788,7 +17791,7 @@
         <v>-1</v>
       </c>
       <c r="B360" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
@@ -17796,23 +17799,23 @@
         <v>-1</v>
       </c>
       <c r="B361" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A362">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B362" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A363">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B363" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
@@ -17820,7 +17823,7 @@
         <v>-1</v>
       </c>
       <c r="B364" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
@@ -17828,7 +17831,7 @@
         <v>-1</v>
       </c>
       <c r="B365" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.25">
@@ -17836,7 +17839,7 @@
         <v>-1</v>
       </c>
       <c r="B366" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
@@ -17844,7 +17847,7 @@
         <v>-1</v>
       </c>
       <c r="B367" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
@@ -17852,7 +17855,7 @@
         <v>-1</v>
       </c>
       <c r="B368" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.25">
@@ -17860,23 +17863,23 @@
         <v>-1</v>
       </c>
       <c r="B369" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A370">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B370" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A371">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B371" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
@@ -17884,23 +17887,23 @@
         <v>-1</v>
       </c>
       <c r="B372" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A373">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B373" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A374">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B374" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
@@ -17908,15 +17911,15 @@
         <v>-1</v>
       </c>
       <c r="B375" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A376">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B376" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
@@ -17924,31 +17927,31 @@
         <v>1</v>
       </c>
       <c r="B377" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A378">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B378" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A379">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B379" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A380">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B380" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
@@ -17956,7 +17959,7 @@
         <v>-1</v>
       </c>
       <c r="B381" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
@@ -17964,7 +17967,7 @@
         <v>-1</v>
       </c>
       <c r="B382" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
@@ -17972,7 +17975,7 @@
         <v>-1</v>
       </c>
       <c r="B383" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
@@ -17980,7 +17983,7 @@
         <v>-1</v>
       </c>
       <c r="B384" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
@@ -17988,7 +17991,7 @@
         <v>-1</v>
       </c>
       <c r="B385" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
@@ -17996,15 +17999,15 @@
         <v>-1</v>
       </c>
       <c r="B386" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A387">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B387" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
@@ -18012,15 +18015,15 @@
         <v>1</v>
       </c>
       <c r="B388" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A389">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B389" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.25">
@@ -18028,7 +18031,7 @@
         <v>-1</v>
       </c>
       <c r="B390" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
@@ -18036,7 +18039,7 @@
         <v>-1</v>
       </c>
       <c r="B391" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
@@ -18044,7 +18047,7 @@
         <v>-1</v>
       </c>
       <c r="B392" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
@@ -18052,7 +18055,7 @@
         <v>-1</v>
       </c>
       <c r="B393" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
@@ -18060,7 +18063,7 @@
         <v>-1</v>
       </c>
       <c r="B394" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
@@ -18068,7 +18071,7 @@
         <v>-1</v>
       </c>
       <c r="B395" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
@@ -18076,7 +18079,7 @@
         <v>-1</v>
       </c>
       <c r="B396" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.25">
@@ -18084,7 +18087,7 @@
         <v>-1</v>
       </c>
       <c r="B397" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.25">
@@ -18092,23 +18095,23 @@
         <v>-1</v>
       </c>
       <c r="B398" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A399">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B399" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A400">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B400" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
@@ -18116,7 +18119,7 @@
         <v>-1</v>
       </c>
       <c r="B401" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.25">
@@ -18124,7 +18127,7 @@
         <v>-1</v>
       </c>
       <c r="B402" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.25">
@@ -18132,14 +18135,22 @@
         <v>-1</v>
       </c>
       <c r="B403" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A404">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B404" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A405">
+        <v>1</v>
+      </c>
+      <c r="B405" t="s">
         <v>1343</v>
       </c>
     </row>
@@ -34138,7 +34149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{923A9D79-A1A9-4F21-A2E5-D563F861F215}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>